<commit_message>
Update mapping new chips IDs
</commit_message>
<xml_diff>
--- a/IDsMapping.xlsx
+++ b/IDsMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roth_\Uni\1.Semester_WS1920\Algorithmen MMI\GitHub\Smart_Kitchen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0063704E-37E6-4F36-94B1-CD495EBEC405}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91B078B-FD2B-475F-BDEE-1E12D51A0D43}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CCBDE61-6562-4498-99E4-B5911D7CAF8A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$B$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$C$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -154,6 +154,36 @@
   </si>
   <si>
     <t>Teigschaber</t>
+  </si>
+  <si>
+    <t>103022550827</t>
+  </si>
+  <si>
+    <t>987535843987</t>
+  </si>
+  <si>
+    <t>786142748451</t>
+  </si>
+  <si>
+    <t>796112435620</t>
+  </si>
+  <si>
+    <t>1064020239013</t>
+  </si>
+  <si>
+    <t>39911334407</t>
+  </si>
+  <si>
+    <t>995451166718</t>
+  </si>
+  <si>
+    <t>858500718555</t>
+  </si>
+  <si>
+    <t>855499759477</t>
+  </si>
+  <si>
+    <t>718631362413</t>
   </si>
 </sst>
 </file>
@@ -525,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D55858-6FAC-4A98-9878-983856C9915C}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C30" sqref="A1:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,7 +693,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
@@ -672,7 +704,9 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
@@ -681,7 +715,9 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
@@ -690,7 +726,9 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
@@ -699,7 +737,9 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="B19" s="3" t="s">
         <v>13</v>
       </c>
@@ -713,7 +753,9 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
+      <c r="A23" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="B23" s="3" t="s">
         <v>24</v>
       </c>
@@ -722,7 +764,9 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="B24" s="3" t="s">
         <v>34</v>
       </c>
@@ -731,7 +775,9 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B25" s="3" t="s">
         <v>26</v>
       </c>
@@ -740,7 +786,9 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
+      <c r="A26" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B26" s="3" t="s">
         <v>27</v>
       </c>
@@ -749,7 +797,9 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
+      <c r="A27" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="B27" s="3" t="s">
         <v>39</v>
       </c>

</xml_diff>